<commit_message>
completed 9 out of 25 sections for probability distributions
</commit_message>
<xml_diff>
--- a/Excel/Statistics for Data Analysis/StatisticsforDataAnalysis-221118-112009/Projects/Pizza_Sales.xlsx
+++ b/Excel/Statistics for Data Analysis/StatisticsforDataAnalysis-221118-112009/Projects/Pizza_Sales.xlsx
@@ -2,43 +2,32 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jorgesoto/Desktop/Maven_Analytics/Excel/Statistics for Data Analysis/StatisticsforDataAnalysis-221118-112009/Projects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82500B8D-AB88-EA45-A7D8-FDC5AEB2A3B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DB57A07-ABCE-674A-89E9-DF7C4BB39D7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="20140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="20140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="orders" sheetId="1" r:id="rId1"/>
+    <sheet name="Dashboard" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">orders!$A$1:$C$359</definedName>
     <definedName name="_xlchart.v1.0" hidden="1">orders!$B$2:$B$359</definedName>
     <definedName name="_xlchart.v1.1" hidden="1">orders!$C$1</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">orders!$C$1</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">orders!$C$2:$C$359</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">orders!$B$2:$B$359</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">orders!$C$1</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">orders!$C$2:$C$359</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">orders!$B$2:$B$359</definedName>
-    <definedName name="_xlchart.v1.16" hidden="1">orders!$C$1</definedName>
-    <definedName name="_xlchart.v1.17" hidden="1">orders!$C$2:$C$359</definedName>
     <definedName name="_xlchart.v1.2" hidden="1">orders!$C$2:$C$359</definedName>
     <definedName name="_xlchart.v1.3" hidden="1">orders!$B$2:$B$359</definedName>
     <definedName name="_xlchart.v1.4" hidden="1">orders!$C$1</definedName>
     <definedName name="_xlchart.v1.5" hidden="1">orders!$C$2:$C$359</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">orders!$B$2:$B$359</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">orders!$C$1</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">orders!$C$2:$C$359</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">orders!$B$2:$B$359</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="29" r:id="rId2"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -57,7 +46,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -210,7 +199,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
-    <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="20" x14ac:knownFonts="1">
     <font>
@@ -718,7 +707,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -726,15 +715,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -780,7 +768,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="26">
+  <dxfs count="4">
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
@@ -789,72 +777,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="0.0000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="169" formatCode="0.00000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="0.000000"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
@@ -887,7 +809,7 @@
   </mc:AlternateContent>
   <c:pivotSource>
     <c:name>[Pizza_Sales.xlsx]orders!PivotTable5</c:name>
-    <c:fmtId val="1"/>
+    <c:fmtId val="3"/>
   </c:pivotSource>
   <c:chart>
     <c:title>
@@ -954,6 +876,114 @@
     <c:pivotFmts>
       <c:pivotFmt>
         <c:idx val="0"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1050" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="bg1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:dLblPos val="inEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="1"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1050" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="bg1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:dLblPos val="inEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="2"/>
         <c:spPr>
           <a:solidFill>
             <a:schemeClr val="accent1"/>
@@ -1153,7 +1183,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-2405-0E48-BEC6-61C7E223F613}"/>
+              <c16:uniqueId val="{00000000-3892-F84C-906A-65969E972390}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1441,13 +1471,125 @@
   </mc:AlternateContent>
   <c:pivotSource>
     <c:name>[Pizza_Sales.xlsx]orders!PivotTable6</c:name>
-    <c:fmtId val="2"/>
+    <c:fmtId val="4"/>
   </c:pivotSource>
   <c:chart>
     <c:autoTitleDeleted val="1"/>
     <c:pivotFmts>
       <c:pivotFmt>
         <c:idx val="0"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="1"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="2"/>
         <c:spPr>
           <a:solidFill>
             <a:schemeClr val="accent1"/>
@@ -1514,7 +1656,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>orders!$R$2</c:f>
+              <c:f>orders!$F$12</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1535,7 +1677,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>orders!$Q$3:$Q$20</c:f>
+              <c:f>orders!$E$13:$E$30</c:f>
               <c:strCache>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
@@ -1594,7 +1736,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>orders!$R$3:$R$20</c:f>
+              <c:f>orders!$F$13:$F$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="17"/>
@@ -1654,7 +1796,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-5B49-984C-AEE0-85E1FA13E6A8}"/>
+              <c16:uniqueId val="{00000000-17CB-9E43-8994-E978DCF559A1}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1678,6 +1820,66 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Pizza</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Sold</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1743,6 +1945,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number of Dasy</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1850,10 +2107,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.15</cx:f>
+        <cx:f>_xlchart.v1.3</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.17</cx:f>
+        <cx:f>_xlchart.v1.5</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -1863,7 +2120,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{A0BF6424-BEFD-334C-93DC-31F7EA157907}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.16</cx:f>
+              <cx:f>_xlchart.v1.4</cx:f>
               <cx:v>Pizzas</cx:v>
             </cx:txData>
           </cx:tx>
@@ -2547,6 +2804,509 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="406">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3061,534 +3821,33 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>50800</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>254000</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>558800</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
+        <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{28241FA4-0299-C280-C88A-5D701CB56F29}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7193B35A-8698-1047-B30A-5221ACED5B5D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -3604,16 +3863,54 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>1174750</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>57</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>122016</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{408A46BD-8EEE-C444-9156-7D6145BF917A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>139700</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
@@ -3622,7 +3919,7 @@
             <xdr:cNvPr id="4" name="Chart 3">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F1958458-F9F3-670C-E92A-28FFCAECE9FF}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1D0058C7-5652-634E-80EB-AC5A31511718}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3634,7 +3931,7 @@
           </xdr:xfrm>
           <a:graphic>
             <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
-              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
             </a:graphicData>
           </a:graphic>
         </xdr:graphicFrame>
@@ -3649,8 +3946,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="5302250" y="6642100"/>
-              <a:ext cx="7512050" cy="4368800"/>
+              <a:off x="7569200" y="1435100"/>
+              <a:ext cx="7537450" cy="4406900"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -3682,38 +3979,74 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>139700</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>28</xdr:col>
-      <xdr:colOff>12700</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Chart 5">
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="TextBox 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{42BBD5B5-EC22-1676-AFA0-887EE5569B37}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AD59A1AD-84CE-A095-4961-DDD7E62CD9BA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="38100" y="0"/>
+          <a:ext cx="6946900" cy="850900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800"/>
+            <a:t>We want</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" baseline="0"/>
+            <a:t> to know how many pizza sales to expect everyday, how much they typically vary, and if they fluctuate by day of the week.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1800"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -5671,8 +6004,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{AA94F1EA-3629-C14A-ADEC-75CD8B7E2758}" name="PivotTable6" cacheId="29" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3" rowHeaderCaption="Day of Week">
-  <location ref="Q2:R20" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{AA94F1EA-3629-C14A-ADEC-75CD8B7E2758}" name="PivotTable6" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="5" rowHeaderCaption="Day of Week">
+  <location ref="E12:F30" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField numFmtId="164" showAll="0"/>
     <pivotField showAll="0">
@@ -5781,12 +6114,21 @@
     <dataField name="Count of Pizzas" fld="2" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="17">
+    <format dxfId="1">
       <pivotArea grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
-  <chartFormats count="1">
+  <chartFormats count="2">
     <chartFormat chart="2" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="2" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -5809,7 +6151,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{96DB2E56-E88A-B649-828D-045E94B55372}" name="PivotTable5" cacheId="29" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2" rowHeaderCaption="Day of Week">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{96DB2E56-E88A-B649-828D-045E94B55372}" name="PivotTable5" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4" rowHeaderCaption="Day of Week">
   <location ref="E2:F10" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField numFmtId="164" showAll="0"/>
@@ -5898,18 +6240,18 @@
     <dataField name="Average Pizza Sales " fld="2" subtotal="average" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="2">
-    <format dxfId="25">
+    <format dxfId="3">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="19">
+    <format dxfId="2">
       <pivotArea grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
-  <chartFormats count="2">
+  <chartFormats count="3">
     <chartFormat chart="0" format="0" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
@@ -5920,6 +6262,15 @@
       </pivotArea>
     </chartFormat>
     <chartFormat chart="1" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="2" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -6238,10 +6589,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R359"/>
+  <dimension ref="A1:P359"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q25" sqref="Q25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6249,12 +6600,13 @@
     <col min="1" max="2" width="12.1640625" customWidth="1"/>
     <col min="5" max="5" width="13.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.1640625" customWidth="1"/>
+    <col min="8" max="8" width="20.1640625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="13.1640625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6264,8 +6616,32 @@
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="I1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N1" t="s">
+        <v>8</v>
+      </c>
+      <c r="O1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P1" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>42005</v>
       </c>
@@ -6281,14 +6657,43 @@
       <c r="F2" t="s">
         <v>11</v>
       </c>
-      <c r="Q2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="R2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="H2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" cm="1">
+        <f t="array" ref="I2">MIN(IF($B$2:$B$359=I1,$C$2:$C$359))</f>
+        <v>102</v>
+      </c>
+      <c r="J2" cm="1">
+        <f t="array" ref="J2">MIN(IF($B$2:$B$359=J1,$C$2:$C$359))</f>
+        <v>80</v>
+      </c>
+      <c r="K2" cm="1">
+        <f t="array" ref="K2">MIN(IF($B$2:$B$359=K1,$C$2:$C$359))</f>
+        <v>82</v>
+      </c>
+      <c r="L2" cm="1">
+        <f t="array" ref="L2">MIN(IF($B$2:$B$359=L1,$C$2:$C$359))</f>
+        <v>113</v>
+      </c>
+      <c r="M2" cm="1">
+        <f t="array" ref="M2">MIN(IF($B$2:$B$359=M1,$C$2:$C$359))</f>
+        <v>125</v>
+      </c>
+      <c r="N2" cm="1">
+        <f t="array" ref="N2">MIN(IF($B$2:$B$359=N1,$C$2:$C$359))</f>
+        <v>95</v>
+      </c>
+      <c r="O2" cm="1">
+        <f t="array" ref="O2">MIN(IF($B$2:$B$359=O1,$C$2:$C$359))</f>
+        <v>77</v>
+      </c>
+      <c r="P2" s="8" cm="1">
+        <f t="array" ref="P2:P6">_xlfn.QUARTILE.INC(C2:C359,_xlfn.SEQUENCE(5,,0,1))</f>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>42006</v>
       </c>
@@ -6301,17 +6706,45 @@
       <c r="E3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3" s="5">
         <v>164.84</v>
       </c>
-      <c r="Q3" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="R3" s="5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="H3" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" cm="1">
+        <f t="array" ref="I3">_xlfn.QUARTILE.INC(IF($B$2:$B$359=I1,$C$2:$C$359),1)</f>
+        <v>125.75</v>
+      </c>
+      <c r="J3" cm="1">
+        <f t="array" ref="J3">_xlfn.QUARTILE.INC(IF($B$2:$B$359=J1,$C$2:$C$359),1)</f>
+        <v>119.75</v>
+      </c>
+      <c r="K3" cm="1">
+        <f t="array" ref="K3">_xlfn.QUARTILE.INC(IF($B$2:$B$359=K1,$C$2:$C$359),1)</f>
+        <v>125.5</v>
+      </c>
+      <c r="L3" cm="1">
+        <f t="array" ref="L3">_xlfn.QUARTILE.INC(IF($B$2:$B$359=L1,$C$2:$C$359),1)</f>
+        <v>125.5</v>
+      </c>
+      <c r="M3" cm="1">
+        <f t="array" ref="M3">_xlfn.QUARTILE.INC(IF($B$2:$B$359=M1,$C$2:$C$359),1)</f>
+        <v>152.25</v>
+      </c>
+      <c r="N3" cm="1">
+        <f t="array" ref="N3">_xlfn.QUARTILE.INC(IF($B$2:$B$359=N1,$C$2:$C$359),1)</f>
+        <v>135.75</v>
+      </c>
+      <c r="O3" cm="1">
+        <f t="array" ref="O3">_xlfn.QUARTILE.INC(IF($B$2:$B$359=O1,$C$2:$C$359),1)</f>
+        <v>105.75</v>
+      </c>
+      <c r="P3" s="8">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>42007</v>
       </c>
@@ -6324,17 +6757,45 @@
       <c r="E4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="5">
         <v>144.09615384615384</v>
       </c>
-      <c r="Q4" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="R4" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="H4" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" s="5" cm="1">
+        <f t="array" ref="I4">MEDIAN(IF($B$2:$B$359=I1,$C$2:$C$359))</f>
+        <v>135.5</v>
+      </c>
+      <c r="J4" s="5" cm="1">
+        <f t="array" ref="J4">MEDIAN(IF($B$2:$B$359=J1,$C$2:$C$359))</f>
+        <v>131.5</v>
+      </c>
+      <c r="K4" s="5" cm="1">
+        <f t="array" ref="K4">MEDIAN(IF($B$2:$B$359=K1,$C$2:$C$359))</f>
+        <v>134.5</v>
+      </c>
+      <c r="L4" s="5" cm="1">
+        <f t="array" ref="L4">MEDIAN(IF($B$2:$B$359=L1,$C$2:$C$359))</f>
+        <v>137.5</v>
+      </c>
+      <c r="M4" s="5" cm="1">
+        <f t="array" ref="M4">MEDIAN(IF($B$2:$B$359=M1,$C$2:$C$359))</f>
+        <v>163</v>
+      </c>
+      <c r="N4" s="5" cm="1">
+        <f t="array" ref="N4">MEDIAN(IF($B$2:$B$359=N1,$C$2:$C$359))</f>
+        <v>142</v>
+      </c>
+      <c r="O4" s="5" cm="1">
+        <f t="array" ref="O4">MEDIAN(IF($B$2:$B$359=O1,$C$2:$C$359))</f>
+        <v>115</v>
+      </c>
+      <c r="P4" s="9">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>42008</v>
       </c>
@@ -6347,17 +6808,45 @@
       <c r="E5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="5">
         <v>143.80769230769232</v>
       </c>
-      <c r="Q5" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="R5" s="5">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="H5" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I5" cm="1">
+        <f t="array" ref="I5">_xlfn.QUARTILE.INC(IF($B$2:$B$359=I1,$C$2:$C$359),3)</f>
+        <v>142.5</v>
+      </c>
+      <c r="J5" cm="1">
+        <f t="array" ref="J5">_xlfn.QUARTILE.INC(IF($B$2:$B$359=J1,$C$2:$C$359),3)</f>
+        <v>144.5</v>
+      </c>
+      <c r="K5" cm="1">
+        <f t="array" ref="K5">_xlfn.QUARTILE.INC(IF($B$2:$B$359=K1,$C$2:$C$359),3)</f>
+        <v>141.25</v>
+      </c>
+      <c r="L5" cm="1">
+        <f t="array" ref="L5">_xlfn.QUARTILE.INC(IF($B$2:$B$359=L1,$C$2:$C$359),3)</f>
+        <v>149.25</v>
+      </c>
+      <c r="M5" cm="1">
+        <f t="array" ref="M5">_xlfn.QUARTILE.INC(IF($B$2:$B$359=M1,$C$2:$C$359),3)</f>
+        <v>175.75</v>
+      </c>
+      <c r="N5" cm="1">
+        <f t="array" ref="N5">_xlfn.QUARTILE.INC(IF($B$2:$B$359=N1,$C$2:$C$359),3)</f>
+        <v>153</v>
+      </c>
+      <c r="O5" cm="1">
+        <f t="array" ref="O5">_xlfn.QUARTILE.INC(IF($B$2:$B$359=O1,$C$2:$C$359),3)</f>
+        <v>127.25</v>
+      </c>
+      <c r="P5" s="8">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>42009</v>
       </c>
@@ -6370,17 +6859,45 @@
       <c r="E6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="5">
         <v>135.10416666666666</v>
       </c>
-      <c r="Q6" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="R6" s="5">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="H6" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="I6" cm="1">
+        <f t="array" ref="I6">MAX(IF($B$2:$B$359=I1,$C$2:$C$359))</f>
+        <v>184</v>
+      </c>
+      <c r="J6" cm="1">
+        <f t="array" ref="J6">MAX(IF($B$2:$B$359=J1,$C$2:$C$359))</f>
+        <v>179</v>
+      </c>
+      <c r="K6" cm="1">
+        <f t="array" ref="K6">MAX(IF($B$2:$B$359=K1,$C$2:$C$359))</f>
+        <v>163</v>
+      </c>
+      <c r="L6" cm="1">
+        <f t="array" ref="L6">MAX(IF($B$2:$B$359=L1,$C$2:$C$359))</f>
+        <v>266</v>
+      </c>
+      <c r="M6" cm="1">
+        <f t="array" ref="M6">MAX(IF($B$2:$B$359=M1,$C$2:$C$359))</f>
+        <v>264</v>
+      </c>
+      <c r="N6" cm="1">
+        <f t="array" ref="N6">MAX(IF($B$2:$B$359=N1,$C$2:$C$359))</f>
+        <v>234</v>
+      </c>
+      <c r="O6" cm="1">
+        <f t="array" ref="O6">MAX(IF($B$2:$B$359=O1,$C$2:$C$359))</f>
+        <v>191</v>
+      </c>
+      <c r="P6" s="8">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>42010</v>
       </c>
@@ -6393,17 +6910,46 @@
       <c r="E7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7" s="5">
         <v>133.57692307692307</v>
       </c>
-      <c r="Q7" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="R7" s="5">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="H7" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="I7">
+        <f>I5-I3</f>
+        <v>16.75</v>
+      </c>
+      <c r="J7">
+        <f t="shared" ref="J7:N7" si="0">J5-J3</f>
+        <v>24.75</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="0"/>
+        <v>15.75</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="0"/>
+        <v>23.75</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="0"/>
+        <v>23.5</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="0"/>
+        <v>17.25</v>
+      </c>
+      <c r="O7">
+        <f>O5-O3</f>
+        <v>21.5</v>
+      </c>
+      <c r="P7" s="8">
+        <f>P5-P3</f>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>42011</v>
       </c>
@@ -6416,17 +6962,46 @@
       <c r="E8" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F8" s="5">
         <v>132.59615384615384</v>
       </c>
-      <c r="Q8" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="R8" s="5">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="H8" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="I8" s="7" cm="1">
+        <f t="array" ref="I8">_xlfn.STDEV.S(IF($B$2:$B$359=I1,$C$2:$C$359))</f>
+        <v>14.48732326763616</v>
+      </c>
+      <c r="J8" s="7" cm="1">
+        <f t="array" ref="J8">_xlfn.STDEV.S(IF($B$2:$B$359=J1,$C$2:$C$359))</f>
+        <v>17.378440119742493</v>
+      </c>
+      <c r="K8" s="7" cm="1">
+        <f t="array" ref="K8">_xlfn.STDEV.S(IF($B$2:$B$359=K1,$C$2:$C$359))</f>
+        <v>15.087127552913687</v>
+      </c>
+      <c r="L8" s="7" cm="1">
+        <f t="array" ref="L8">_xlfn.STDEV.S(IF($B$2:$B$359=L1,$C$2:$C$359))</f>
+        <v>29.765777468354951</v>
+      </c>
+      <c r="M8" s="7" cm="1">
+        <f t="array" ref="M8">_xlfn.STDEV.S(IF($B$2:$B$359=M1,$C$2:$C$359))</f>
+        <v>23.654278639586181</v>
+      </c>
+      <c r="N8" s="7" cm="1">
+        <f t="array" ref="N8">_xlfn.STDEV.S(IF($B$2:$B$359=N1,$C$2:$C$359))</f>
+        <v>19.225452507879506</v>
+      </c>
+      <c r="O8" s="7" cm="1">
+        <f t="array" ref="O8">_xlfn.STDEV.S(IF($B$2:$B$359=O1,$C$2:$C$359))</f>
+        <v>18.318974906608677</v>
+      </c>
+      <c r="P8" s="10">
+        <f>_xlfn.STDEV.S(C2:C359)</f>
+        <v>24.428669026957198</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>42012</v>
       </c>
@@ -6439,17 +7014,46 @@
       <c r="E9" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="6">
+      <c r="F9" s="5">
         <v>116.05769230769231</v>
       </c>
-      <c r="Q9" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="R9" s="5">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="H9" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I9" s="7">
+        <f>AVERAGEIFS($C$2:$C$359,$B$2:$B$359,I1)</f>
+        <v>135.10416666666666</v>
+      </c>
+      <c r="J9" s="5">
+        <f t="shared" ref="J9:O9" si="1">AVERAGEIFS($C$2:$C$359,$B$2:$B$359,J1)</f>
+        <v>132.59615384615384</v>
+      </c>
+      <c r="K9" s="5">
+        <f t="shared" si="1"/>
+        <v>133.57692307692307</v>
+      </c>
+      <c r="L9" s="5">
+        <f t="shared" si="1"/>
+        <v>143.80769230769232</v>
+      </c>
+      <c r="M9" s="5">
+        <f t="shared" si="1"/>
+        <v>164.84</v>
+      </c>
+      <c r="N9" s="5">
+        <f t="shared" si="1"/>
+        <v>144.09615384615384</v>
+      </c>
+      <c r="O9" s="5">
+        <f t="shared" si="1"/>
+        <v>116.05769230769231</v>
+      </c>
+      <c r="P9" s="9">
+        <f>AVERAGE(C2:C359)</f>
+        <v>138.47486033519553</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>42013</v>
       </c>
@@ -6462,17 +7066,46 @@
       <c r="E10" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F10" s="6">
+      <c r="F10" s="5">
         <v>138.47486033519553</v>
       </c>
-      <c r="Q10" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="R10" s="5">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="H10" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="I10">
+        <f>I8/I9</f>
+        <v>0.10723076589769248</v>
+      </c>
+      <c r="J10">
+        <f t="shared" ref="J10:O10" si="2">J8/J9</f>
+        <v>0.13106292766158226</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="2"/>
+        <v>0.11294711096336191</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="2"/>
+        <v>0.20698320785697477</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="2"/>
+        <v>0.14349841445999867</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="2"/>
+        <v>0.13342099698515072</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="2"/>
+        <v>0.15784369430715015</v>
+      </c>
+      <c r="P10" s="8">
+        <f>P8/P9</f>
+        <v>0.17641230305504249</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>42014</v>
       </c>
@@ -6482,14 +7115,8 @@
       <c r="C11">
         <v>146</v>
       </c>
-      <c r="Q11" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="R11" s="5">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>42015</v>
       </c>
@@ -6499,14 +7126,14 @@
       <c r="C12">
         <v>116</v>
       </c>
-      <c r="Q12" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="R12" s="5">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="E12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>42016</v>
       </c>
@@ -6516,14 +7143,14 @@
       <c r="C13">
         <v>119</v>
       </c>
-      <c r="Q13" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="R13" s="5">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="E13" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>42017</v>
       </c>
@@ -6533,14 +7160,14 @@
       <c r="C14">
         <v>120</v>
       </c>
-      <c r="Q14" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="R14" s="5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="E14" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>42018</v>
       </c>
@@ -6550,14 +7177,14 @@
       <c r="C15">
         <v>150</v>
       </c>
-      <c r="Q15" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="R15" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="E15" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F15">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>42019</v>
       </c>
@@ -6567,14 +7194,14 @@
       <c r="C16">
         <v>123</v>
       </c>
-      <c r="Q16" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="R16" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="E16" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F16">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>42020</v>
       </c>
@@ -6584,14 +7211,14 @@
       <c r="C17">
         <v>158</v>
       </c>
-      <c r="Q17" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="R17" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="E17" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F17">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>42021</v>
       </c>
@@ -6601,14 +7228,14 @@
       <c r="C18">
         <v>125</v>
       </c>
-      <c r="Q18" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="R18" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="E18" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F18">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>42022</v>
       </c>
@@ -6618,14 +7245,14 @@
       <c r="C19">
         <v>122</v>
       </c>
-      <c r="Q19" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="R19" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="E19" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F19">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>42023</v>
       </c>
@@ -6635,14 +7262,14 @@
       <c r="C20">
         <v>142</v>
       </c>
-      <c r="Q20" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="R20" s="6">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="E20" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F20">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>42024</v>
       </c>
@@ -6652,8 +7279,14 @@
       <c r="C21">
         <v>143</v>
       </c>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="E21" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F21">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>42025</v>
       </c>
@@ -6663,8 +7296,14 @@
       <c r="C22">
         <v>129</v>
       </c>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="E22" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F22">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>42026</v>
       </c>
@@ -6674,8 +7313,14 @@
       <c r="C23">
         <v>158</v>
       </c>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="E23" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F23">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>42027</v>
       </c>
@@ -6685,8 +7330,14 @@
       <c r="C24">
         <v>152</v>
       </c>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="E24" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F24">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>42028</v>
       </c>
@@ -6696,32 +7347,14 @@
       <c r="C25">
         <v>142</v>
       </c>
-      <c r="H25" t="s">
-        <v>3</v>
-      </c>
-      <c r="I25" t="s">
-        <v>4</v>
-      </c>
-      <c r="J25" t="s">
-        <v>5</v>
-      </c>
-      <c r="K25" t="s">
-        <v>6</v>
-      </c>
-      <c r="L25" t="s">
-        <v>7</v>
-      </c>
-      <c r="M25" t="s">
-        <v>8</v>
-      </c>
-      <c r="N25" t="s">
-        <v>9</v>
-      </c>
-      <c r="O25" s="9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="E25" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>42029</v>
       </c>
@@ -6731,43 +7364,14 @@
       <c r="C26">
         <v>102</v>
       </c>
-      <c r="G26" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H26" cm="1">
-        <f t="array" ref="H26">MIN(IF($B$2:$B$359=H25,$C$2:$C$359))</f>
-        <v>102</v>
-      </c>
-      <c r="I26" cm="1">
-        <f t="array" ref="I26">MIN(IF($B$2:$B$359=I25,$C$2:$C$359))</f>
-        <v>80</v>
-      </c>
-      <c r="J26" cm="1">
-        <f t="array" ref="J26">MIN(IF($B$2:$B$359=J25,$C$2:$C$359))</f>
-        <v>82</v>
-      </c>
-      <c r="K26" cm="1">
-        <f t="array" ref="K26">MIN(IF($B$2:$B$359=K25,$C$2:$C$359))</f>
-        <v>113</v>
-      </c>
-      <c r="L26" cm="1">
-        <f t="array" ref="L26">MIN(IF($B$2:$B$359=L25,$C$2:$C$359))</f>
-        <v>125</v>
-      </c>
-      <c r="M26" cm="1">
-        <f t="array" ref="M26">MIN(IF($B$2:$B$359=M25,$C$2:$C$359))</f>
-        <v>95</v>
-      </c>
-      <c r="N26" cm="1">
-        <f t="array" ref="N26">MIN(IF($B$2:$B$359=N25,$C$2:$C$359))</f>
-        <v>77</v>
-      </c>
-      <c r="O26" s="9" cm="1">
-        <f t="array" ref="O26:O30">_xlfn.QUARTILE.INC(C2:C359,_xlfn.SEQUENCE(5,,0,1))</f>
-        <v>77</v>
-      </c>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="E26" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>42030</v>
       </c>
@@ -6777,43 +7381,14 @@
       <c r="C27">
         <v>113</v>
       </c>
-      <c r="E27" s="7"/>
-      <c r="G27" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="H27" cm="1">
-        <f t="array" ref="H27">_xlfn.QUARTILE.INC(IF($B$2:$B$359=H25,$C$2:$C$359),1)</f>
-        <v>125.75</v>
-      </c>
-      <c r="I27" cm="1">
-        <f t="array" ref="I27">_xlfn.QUARTILE.INC(IF($B$2:$B$359=I25,$C$2:$C$359),1)</f>
-        <v>119.75</v>
-      </c>
-      <c r="J27" cm="1">
-        <f t="array" ref="J27">_xlfn.QUARTILE.INC(IF($B$2:$B$359=J25,$C$2:$C$359),1)</f>
-        <v>125.5</v>
-      </c>
-      <c r="K27" cm="1">
-        <f t="array" ref="K27">_xlfn.QUARTILE.INC(IF($B$2:$B$359=K25,$C$2:$C$359),1)</f>
-        <v>125.5</v>
-      </c>
-      <c r="L27" cm="1">
-        <f t="array" ref="L27">_xlfn.QUARTILE.INC(IF($B$2:$B$359=L25,$C$2:$C$359),1)</f>
-        <v>152.25</v>
-      </c>
-      <c r="M27" cm="1">
-        <f t="array" ref="M27">_xlfn.QUARTILE.INC(IF($B$2:$B$359=M25,$C$2:$C$359),1)</f>
-        <v>135.75</v>
-      </c>
-      <c r="N27" cm="1">
-        <f t="array" ref="N27">_xlfn.QUARTILE.INC(IF($B$2:$B$359=N25,$C$2:$C$359),1)</f>
-        <v>105.75</v>
-      </c>
-      <c r="O27" s="9">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="E27" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>42031</v>
       </c>
@@ -6823,43 +7398,14 @@
       <c r="C28">
         <v>151</v>
       </c>
-      <c r="E28" s="7"/>
-      <c r="G28" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="H28" s="6" cm="1">
-        <f t="array" ref="H28">MEDIAN(IF($B$2:$B$359=H25,$C$2:$C$359))</f>
-        <v>135.5</v>
-      </c>
-      <c r="I28" s="6" cm="1">
-        <f t="array" ref="I28">MEDIAN(IF($B$2:$B$359=I25,$C$2:$C$359))</f>
-        <v>131.5</v>
-      </c>
-      <c r="J28" s="6" cm="1">
-        <f t="array" ref="J28">MEDIAN(IF($B$2:$B$359=J25,$C$2:$C$359))</f>
-        <v>134.5</v>
-      </c>
-      <c r="K28" s="6" cm="1">
-        <f t="array" ref="K28">MEDIAN(IF($B$2:$B$359=K25,$C$2:$C$359))</f>
-        <v>137.5</v>
-      </c>
-      <c r="L28" s="6" cm="1">
-        <f t="array" ref="L28">MEDIAN(IF($B$2:$B$359=L25,$C$2:$C$359))</f>
-        <v>163</v>
-      </c>
-      <c r="M28" s="6" cm="1">
-        <f t="array" ref="M28">MEDIAN(IF($B$2:$B$359=M25,$C$2:$C$359))</f>
-        <v>142</v>
-      </c>
-      <c r="N28" s="6" cm="1">
-        <f t="array" ref="N28">MEDIAN(IF($B$2:$B$359=N25,$C$2:$C$359))</f>
-        <v>115</v>
-      </c>
-      <c r="O28" s="10">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="E28" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>42032</v>
       </c>
@@ -6869,43 +7415,14 @@
       <c r="C29">
         <v>118</v>
       </c>
-      <c r="E29" s="7"/>
-      <c r="G29" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="H29" cm="1">
-        <f t="array" ref="H29">_xlfn.QUARTILE.INC(IF($B$2:$B$359=H25,$C$2:$C$359),3)</f>
-        <v>142.5</v>
-      </c>
-      <c r="I29" cm="1">
-        <f t="array" ref="I29">_xlfn.QUARTILE.INC(IF($B$2:$B$359=I25,$C$2:$C$359),3)</f>
-        <v>144.5</v>
-      </c>
-      <c r="J29" cm="1">
-        <f t="array" ref="J29">_xlfn.QUARTILE.INC(IF($B$2:$B$359=J25,$C$2:$C$359),3)</f>
-        <v>141.25</v>
-      </c>
-      <c r="K29" cm="1">
-        <f t="array" ref="K29">_xlfn.QUARTILE.INC(IF($B$2:$B$359=K25,$C$2:$C$359),3)</f>
-        <v>149.25</v>
-      </c>
-      <c r="L29" cm="1">
-        <f t="array" ref="L29">_xlfn.QUARTILE.INC(IF($B$2:$B$359=L25,$C$2:$C$359),3)</f>
-        <v>175.75</v>
-      </c>
-      <c r="M29" cm="1">
-        <f t="array" ref="M29">_xlfn.QUARTILE.INC(IF($B$2:$B$359=M25,$C$2:$C$359),3)</f>
-        <v>153</v>
-      </c>
-      <c r="N29" cm="1">
-        <f t="array" ref="N29">_xlfn.QUARTILE.INC(IF($B$2:$B$359=N25,$C$2:$C$359),3)</f>
-        <v>127.25</v>
-      </c>
-      <c r="O29" s="9">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="E29" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>42033</v>
       </c>
@@ -6915,43 +7432,14 @@
       <c r="C30">
         <v>119</v>
       </c>
-      <c r="E30" s="7"/>
-      <c r="G30" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="H30" cm="1">
-        <f t="array" ref="H30">MAX(IF($B$2:$B$359=H25,$C$2:$C$359))</f>
-        <v>184</v>
-      </c>
-      <c r="I30" cm="1">
-        <f t="array" ref="I30">MAX(IF($B$2:$B$359=I25,$C$2:$C$359))</f>
-        <v>179</v>
-      </c>
-      <c r="J30" cm="1">
-        <f t="array" ref="J30">MAX(IF($B$2:$B$359=J25,$C$2:$C$359))</f>
-        <v>163</v>
-      </c>
-      <c r="K30" cm="1">
-        <f t="array" ref="K30">MAX(IF($B$2:$B$359=K25,$C$2:$C$359))</f>
-        <v>266</v>
-      </c>
-      <c r="L30" cm="1">
-        <f t="array" ref="L30">MAX(IF($B$2:$B$359=L25,$C$2:$C$359))</f>
-        <v>264</v>
-      </c>
-      <c r="M30" cm="1">
-        <f t="array" ref="M30">MAX(IF($B$2:$B$359=M25,$C$2:$C$359))</f>
-        <v>234</v>
-      </c>
-      <c r="N30" cm="1">
-        <f t="array" ref="N30">MAX(IF($B$2:$B$359=N25,$C$2:$C$359))</f>
-        <v>191</v>
-      </c>
-      <c r="O30" s="9">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="E30" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F30" s="5">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>42034</v>
       </c>
@@ -6961,44 +7449,9 @@
       <c r="C31">
         <v>138</v>
       </c>
-      <c r="E31" s="7"/>
-      <c r="G31" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="H31">
-        <f>H29-H27</f>
-        <v>16.75</v>
-      </c>
-      <c r="I31">
-        <f t="shared" ref="I31:N31" si="0">I29-I27</f>
-        <v>24.75</v>
-      </c>
-      <c r="J31">
-        <f t="shared" si="0"/>
-        <v>15.75</v>
-      </c>
-      <c r="K31">
-        <f t="shared" si="0"/>
-        <v>23.75</v>
-      </c>
-      <c r="L31">
-        <f t="shared" si="0"/>
-        <v>23.5</v>
-      </c>
-      <c r="M31">
-        <f t="shared" si="0"/>
-        <v>17.25</v>
-      </c>
-      <c r="N31">
-        <f>N29-N27</f>
-        <v>21.5</v>
-      </c>
-      <c r="O31" s="9">
-        <f>O29-O27</f>
-        <v>26</v>
-      </c>
-    </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="E31" s="6"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>42035</v>
       </c>
@@ -7008,44 +7461,9 @@
       <c r="C32">
         <v>145</v>
       </c>
-      <c r="E32" s="7"/>
-      <c r="G32" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="H32" s="8" cm="1">
-        <f t="array" ref="H32">_xlfn.STDEV.S(IF($B$2:$B$359=H25,$C$2:$C$359))</f>
-        <v>14.48732326763616</v>
-      </c>
-      <c r="I32" s="8" cm="1">
-        <f t="array" ref="I32">_xlfn.STDEV.S(IF($B$2:$B$359=I25,$C$2:$C$359))</f>
-        <v>17.378440119742493</v>
-      </c>
-      <c r="J32" s="8" cm="1">
-        <f t="array" ref="J32">_xlfn.STDEV.S(IF($B$2:$B$359=J25,$C$2:$C$359))</f>
-        <v>15.087127552913687</v>
-      </c>
-      <c r="K32" s="8" cm="1">
-        <f t="array" ref="K32">_xlfn.STDEV.S(IF($B$2:$B$359=K25,$C$2:$C$359))</f>
-        <v>29.765777468354951</v>
-      </c>
-      <c r="L32" s="8" cm="1">
-        <f t="array" ref="L32">_xlfn.STDEV.S(IF($B$2:$B$359=L25,$C$2:$C$359))</f>
-        <v>23.654278639586181</v>
-      </c>
-      <c r="M32" s="8" cm="1">
-        <f t="array" ref="M32">_xlfn.STDEV.S(IF($B$2:$B$359=M25,$C$2:$C$359))</f>
-        <v>19.225452507879506</v>
-      </c>
-      <c r="N32" s="8" cm="1">
-        <f t="array" ref="N32">_xlfn.STDEV.S(IF($B$2:$B$359=N25,$C$2:$C$359))</f>
-        <v>18.318974906608677</v>
-      </c>
-      <c r="O32" s="11">
-        <f>_xlfn.STDEV.S(C2:C359)</f>
-        <v>24.428669026957198</v>
-      </c>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="E32" s="6"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>42036</v>
       </c>
@@ -7055,43 +7473,8 @@
       <c r="C33">
         <v>191</v>
       </c>
-      <c r="G33" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="H33" s="8">
-        <f>AVERAGEIFS($C$2:$C$359,$B$2:$B$359,H25)</f>
-        <v>135.10416666666666</v>
-      </c>
-      <c r="I33" s="6">
-        <f t="shared" ref="I33:N33" si="1">AVERAGEIFS($C$2:$C$359,$B$2:$B$359,I25)</f>
-        <v>132.59615384615384</v>
-      </c>
-      <c r="J33" s="6">
-        <f t="shared" si="1"/>
-        <v>133.57692307692307</v>
-      </c>
-      <c r="K33" s="6">
-        <f t="shared" si="1"/>
-        <v>143.80769230769232</v>
-      </c>
-      <c r="L33" s="6">
-        <f t="shared" si="1"/>
-        <v>164.84</v>
-      </c>
-      <c r="M33" s="6">
-        <f t="shared" si="1"/>
-        <v>144.09615384615384</v>
-      </c>
-      <c r="N33" s="6">
-        <f t="shared" si="1"/>
-        <v>116.05769230769231</v>
-      </c>
-      <c r="O33" s="10">
-        <f>AVERAGE(C2:C359)</f>
-        <v>138.47486033519553</v>
-      </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>42037</v>
       </c>
@@ -7101,43 +7484,8 @@
       <c r="C34">
         <v>145</v>
       </c>
-      <c r="G34" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="H34">
-        <f>H32/H33</f>
-        <v>0.10723076589769248</v>
-      </c>
-      <c r="I34">
-        <f t="shared" ref="I34:O34" si="2">I32/I33</f>
-        <v>0.13106292766158226</v>
-      </c>
-      <c r="J34">
-        <f t="shared" si="2"/>
-        <v>0.11294711096336191</v>
-      </c>
-      <c r="K34">
-        <f t="shared" si="2"/>
-        <v>0.20698320785697477</v>
-      </c>
-      <c r="L34">
-        <f t="shared" si="2"/>
-        <v>0.14349841445999867</v>
-      </c>
-      <c r="M34">
-        <f t="shared" si="2"/>
-        <v>0.13342099698515072</v>
-      </c>
-      <c r="N34">
-        <f t="shared" si="2"/>
-        <v>0.15784369430715015</v>
-      </c>
-      <c r="O34" s="9">
-        <f>O32/O33</f>
-        <v>0.17641230305504249</v>
-      </c>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
         <v>42038</v>
       </c>
@@ -7148,7 +7496,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <v>42039</v>
       </c>
@@ -7159,7 +7507,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
         <v>42040</v>
       </c>
@@ -7170,7 +7518,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
         <v>42041</v>
       </c>
@@ -7181,7 +7529,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <v>42042</v>
       </c>
@@ -7192,7 +7540,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <v>42043</v>
       </c>
@@ -7203,7 +7551,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
         <v>42044</v>
       </c>
@@ -7214,7 +7562,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
         <v>42045</v>
       </c>
@@ -7225,7 +7573,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
         <v>42046</v>
       </c>
@@ -7236,7 +7584,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
         <v>42047</v>
       </c>
@@ -7247,7 +7595,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
         <v>42048</v>
       </c>
@@ -7258,7 +7606,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
         <v>42049</v>
       </c>
@@ -7269,7 +7617,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
         <v>42050</v>
       </c>
@@ -7280,7 +7628,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
         <v>42051</v>
       </c>
@@ -10715,6 +11063,20 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66C35B08-498B-5244-84EC-3A235887BD10}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>